<commit_message>
Finish evaluation component Prettify dissertation remove tools which aren't going to be distributed
git-svn-id: http://svn.pling.org.uk/ternip/trunk@1938 046eaa17-6a8d-4e70-a5e5-287f5f62e04c
</commit_message>
<xml_diff>
--- a/docs/performance-vs-gutime.xlsx
+++ b/docs/performance-vs-gutime.xlsx
@@ -47,6 +47,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -110,6 +113,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +418,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" ref="C3:C15" si="0">AVERAGE(D4:H4)</f>
+        <f t="shared" ref="C4:C8" si="0">AVERAGE(D4:H4)</f>
         <v>50.64011509086</v>
       </c>
       <c r="D4">
@@ -560,7 +564,7 @@
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>5.0752889911920001</v>
       </c>

</xml_diff>